<commit_message>
developed web application structure
</commit_message>
<xml_diff>
--- a/Costing_Sheet.xlsx
+++ b/Costing_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5E5FFC-5857-4400-8E21-A5BBFEBCDDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90012E10-210A-46B4-B90E-1300D47350E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="176">
   <si>
     <t>Thickness</t>
   </si>
@@ -583,6 +583,33 @@
   </si>
   <si>
     <t>Retail</t>
+  </si>
+  <si>
+    <t>ProRate</t>
+  </si>
+  <si>
+    <t>ReRate</t>
+  </si>
+  <si>
+    <t>Labour</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transport </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(Default: 350)</t>
+    </r>
+  </si>
+  <si>
+    <t>Margin 25%</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1476,75 +1503,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1571,7 +1533,68 @@
     <xf numFmtId="0" fontId="12" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2013,8 +2036,8 @@
   </sheetPr>
   <dimension ref="A1:V1012"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" zoomScale="61" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2094,8 +2117,8 @@
       <c r="V2" s="30"/>
     </row>
     <row r="3" spans="1:22" ht="37.200000000000003" customHeight="1">
-      <c r="A3" s="109"/>
-      <c r="B3" s="110"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
       <c r="C3" s="34" t="s">
         <v>4</v>
       </c>
@@ -2124,18 +2147,18 @@
       <c r="V3" s="30"/>
     </row>
     <row r="4" spans="1:22" ht="46.8" customHeight="1" thickBot="1">
-      <c r="A4" s="112"/>
-      <c r="B4" s="113"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="121"/>
       <c r="C4" s="38">
         <f>E37</f>
-        <v>6305.5613100899982</v>
+        <v>47883.688172669994</v>
       </c>
       <c r="D4" s="39">
         <v>40</v>
       </c>
       <c r="E4" s="40">
         <f>((100-D4)/100)*C4</f>
-        <v>3783.3367860539988</v>
+        <v>28730.212903601994</v>
       </c>
       <c r="F4" s="37"/>
       <c r="G4" s="30"/>
@@ -2156,21 +2179,21 @@
       <c r="V4" s="30"/>
     </row>
     <row r="5" spans="1:22" ht="13.2">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="116" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="41" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="42">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D5" s="43">
         <v>0.13</v>
       </c>
       <c r="E5" s="44">
         <f>C5*D5*F2</f>
-        <v>561.6</v>
+        <v>7300.8</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="73" t="s">
@@ -2205,7 +2228,7 @@
       <c r="T5" s="30"/>
     </row>
     <row r="6" spans="1:22" ht="13.2">
-      <c r="A6" s="94"/>
+      <c r="A6" s="117"/>
       <c r="B6" s="45" t="s">
         <v>9</v>
       </c>
@@ -2243,7 +2266,7 @@
       <c r="T6" s="30"/>
     </row>
     <row r="7" spans="1:22" ht="13.2">
-      <c r="A7" s="94"/>
+      <c r="A7" s="117"/>
       <c r="B7" s="45" t="s">
         <v>10</v>
       </c>
@@ -2289,7 +2312,7 @@
       <c r="T7" s="30"/>
     </row>
     <row r="8" spans="1:22" ht="13.2">
-      <c r="A8" s="94"/>
+      <c r="A8" s="117"/>
       <c r="B8" s="45" t="s">
         <v>11</v>
       </c>
@@ -2333,7 +2356,7 @@
       <c r="T8" s="30"/>
     </row>
     <row r="9" spans="1:22" ht="13.2">
-      <c r="A9" s="94"/>
+      <c r="A9" s="117"/>
       <c r="B9" s="45" t="s">
         <v>123</v>
       </c>
@@ -2376,7 +2399,7 @@
       <c r="T9" s="30"/>
     </row>
     <row r="10" spans="1:22" ht="13.2">
-      <c r="A10" s="94"/>
+      <c r="A10" s="117"/>
       <c r="B10" s="45" t="s">
         <v>13</v>
       </c>
@@ -2413,7 +2436,7 @@
       <c r="T10" s="30"/>
     </row>
     <row r="11" spans="1:22" ht="13.2">
-      <c r="A11" s="94"/>
+      <c r="A11" s="117"/>
       <c r="B11" s="45" t="s">
         <v>14</v>
       </c>
@@ -2452,7 +2475,7 @@
       <c r="T11" s="30"/>
     </row>
     <row r="12" spans="1:22" ht="13.2">
-      <c r="A12" s="94"/>
+      <c r="A12" s="117"/>
       <c r="B12" s="45" t="s">
         <v>124</v>
       </c>
@@ -2492,7 +2515,7 @@
       <c r="T12" s="30"/>
     </row>
     <row r="13" spans="1:22" ht="13.2">
-      <c r="A13" s="94"/>
+      <c r="A13" s="117"/>
       <c r="B13" s="45" t="s">
         <v>125</v>
       </c>
@@ -2532,7 +2555,7 @@
       <c r="T13" s="30"/>
     </row>
     <row r="14" spans="1:22" ht="13.2">
-      <c r="A14" s="94"/>
+      <c r="A14" s="117"/>
       <c r="B14" s="45" t="s">
         <v>126</v>
       </c>
@@ -2574,12 +2597,12 @@
       <c r="T14" s="30"/>
     </row>
     <row r="15" spans="1:22" ht="13.2">
-      <c r="A15" s="94"/>
+      <c r="A15" s="117"/>
       <c r="B15" s="45" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="46">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D15" s="47">
         <f>Working!O14</f>
@@ -2587,7 +2610,7 @@
       </c>
       <c r="E15" s="48">
         <f t="shared" si="0"/>
-        <v>352</v>
+        <v>1408</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="4">
@@ -2616,7 +2639,7 @@
       <c r="T15" s="30"/>
     </row>
     <row r="16" spans="1:22" ht="13.2">
-      <c r="A16" s="95"/>
+      <c r="A16" s="118"/>
       <c r="B16" s="45" t="s">
         <v>17</v>
       </c>
@@ -2655,7 +2678,7 @@
       <c r="T16" s="30"/>
     </row>
     <row r="17" spans="1:22" ht="13.2">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="119" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="45" t="s">
@@ -2699,18 +2722,20 @@
       <c r="T17" s="30"/>
     </row>
     <row r="18" spans="1:22" ht="13.2">
-      <c r="A18" s="94"/>
+      <c r="A18" s="117"/>
       <c r="B18" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="46"/>
+      <c r="C18" s="46">
+        <v>6</v>
+      </c>
       <c r="D18" s="47">
         <f>Working!O15</f>
         <v>0.16203703703703703</v>
       </c>
       <c r="E18" s="48">
         <f>F2*D18*2*C18</f>
-        <v>0</v>
+        <v>4200</v>
       </c>
       <c r="F18" s="37"/>
       <c r="G18" s="4">
@@ -2741,7 +2766,7 @@
       <c r="T18" s="30"/>
     </row>
     <row r="19" spans="1:22" ht="13.2">
-      <c r="A19" s="94"/>
+      <c r="A19" s="117"/>
       <c r="B19" s="45" t="s">
         <v>21</v>
       </c>
@@ -2780,7 +2805,7 @@
       <c r="T19" s="30"/>
     </row>
     <row r="20" spans="1:22" ht="13.2">
-      <c r="A20" s="95"/>
+      <c r="A20" s="118"/>
       <c r="B20" s="45" t="s">
         <v>22</v>
       </c>
@@ -2821,14 +2846,14 @@
       <c r="T20" s="30"/>
     </row>
     <row r="21" spans="1:22" ht="13.2">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="119" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="46">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D21" s="47">
         <f>Working!O19</f>
@@ -2836,7 +2861,7 @@
       </c>
       <c r="E21" s="48">
         <f>D21*F2*C21*2</f>
-        <v>213.15789473684211</v>
+        <v>2344.7368421052633</v>
       </c>
       <c r="F21" s="37"/>
       <c r="G21" s="4">
@@ -2865,7 +2890,7 @@
       <c r="T21" s="30"/>
     </row>
     <row r="22" spans="1:22" ht="13.2">
-      <c r="A22" s="94"/>
+      <c r="A22" s="117"/>
       <c r="B22" s="45" t="s">
         <v>25</v>
       </c>
@@ -2907,7 +2932,7 @@
       <c r="T22" s="30"/>
     </row>
     <row r="23" spans="1:22" ht="13.2">
-      <c r="A23" s="95"/>
+      <c r="A23" s="118"/>
       <c r="B23" s="45" t="s">
         <v>26</v>
       </c>
@@ -2948,7 +2973,7 @@
       <c r="T23" s="30"/>
     </row>
     <row r="24" spans="1:22" ht="13.2">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="119" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="45" t="s">
@@ -2991,7 +3016,7 @@
       <c r="T24" s="30"/>
     </row>
     <row r="25" spans="1:22" ht="13.2">
-      <c r="A25" s="95"/>
+      <c r="A25" s="118"/>
       <c r="B25" s="45" t="s">
         <v>30</v>
       </c>
@@ -3033,7 +3058,7 @@
       <c r="T25" s="30"/>
     </row>
     <row r="26" spans="1:22" ht="13.2">
-      <c r="A26" s="93" t="s">
+      <c r="A26" s="119" t="s">
         <v>31</v>
       </c>
       <c r="B26" s="45" t="s">
@@ -3071,7 +3096,7 @@
       <c r="T26" s="30"/>
     </row>
     <row r="27" spans="1:22" ht="13.2">
-      <c r="A27" s="95"/>
+      <c r="A27" s="118"/>
       <c r="B27" s="45" t="s">
         <v>33</v>
       </c>
@@ -3114,15 +3139,15 @@
       <c r="T27" s="30"/>
     </row>
     <row r="28" spans="1:22" ht="17.399999999999999" customHeight="1">
-      <c r="A28" s="98" t="s">
+      <c r="A28" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="99"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="97"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115"/>
       <c r="E28" s="52">
         <f>SUM(E5:E27)</f>
-        <v>1805.0736842105262</v>
+        <v>15931.852631578948</v>
       </c>
       <c r="F28" s="37"/>
       <c r="G28" s="4">
@@ -3153,16 +3178,16 @@
       <c r="T28" s="30"/>
     </row>
     <row r="29" spans="1:22" ht="13.2">
-      <c r="A29" s="93" t="s">
+      <c r="A29" s="119" t="s">
         <v>35</v>
       </c>
       <c r="B29" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="101">
+      <c r="C29" s="124">
         <v>1.6E-2</v>
       </c>
-      <c r="D29" s="97"/>
+      <c r="D29" s="115"/>
       <c r="E29" s="48">
         <f>C2*D2*E2*C29</f>
         <v>34.56</v>
@@ -3194,14 +3219,14 @@
       <c r="V29" s="30"/>
     </row>
     <row r="30" spans="1:22" ht="13.2">
-      <c r="A30" s="94"/>
+      <c r="A30" s="117"/>
       <c r="B30" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="96">
+      <c r="C30" s="122">
         <v>350</v>
       </c>
-      <c r="D30" s="97"/>
+      <c r="D30" s="115"/>
       <c r="E30" s="48">
         <f>C30</f>
         <v>350</v>
@@ -3233,17 +3258,17 @@
       <c r="V30" s="30"/>
     </row>
     <row r="31" spans="1:22" ht="13.2">
-      <c r="A31" s="94"/>
+      <c r="A31" s="117"/>
       <c r="B31" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="96">
+      <c r="C31" s="122">
         <v>4</v>
       </c>
-      <c r="D31" s="97"/>
+      <c r="D31" s="115"/>
       <c r="E31" s="48">
         <f>C31/100*E28</f>
-        <v>72.20294736842105</v>
+        <v>637.27410526315794</v>
       </c>
       <c r="F31" s="37"/>
       <c r="G31" s="4">
@@ -3268,17 +3293,17 @@
       <c r="V31" s="30"/>
     </row>
     <row r="32" spans="1:22" ht="13.2">
-      <c r="A32" s="95"/>
+      <c r="A32" s="118"/>
       <c r="B32" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="96">
+      <c r="C32" s="122">
         <v>10</v>
       </c>
-      <c r="D32" s="97"/>
+      <c r="D32" s="115"/>
       <c r="E32" s="48">
         <f>C32/100*E28</f>
-        <v>180.50736842105263</v>
+        <v>1593.185263157895</v>
       </c>
       <c r="F32" s="37"/>
       <c r="G32" s="4">
@@ -3302,15 +3327,15 @@
       <c r="V32" s="30"/>
     </row>
     <row r="33" spans="1:22" ht="16.8" customHeight="1">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="99"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="97"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="115"/>
       <c r="E33" s="52">
         <f>SUM(E28:E32)</f>
-        <v>2442.3439999999996</v>
+        <v>18546.871999999999</v>
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="4">
@@ -3334,19 +3359,19 @@
       <c r="V33" s="30"/>
     </row>
     <row r="34" spans="1:22" ht="13.2">
-      <c r="A34" s="93" t="s">
+      <c r="A34" s="119" t="s">
         <v>41</v>
       </c>
       <c r="B34" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="100">
+      <c r="C34" s="123">
         <v>25</v>
       </c>
-      <c r="D34" s="97"/>
+      <c r="D34" s="115"/>
       <c r="E34" s="48">
         <f>(1+(C34/100))*E33</f>
-        <v>3052.9299999999994</v>
+        <v>23183.59</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="30"/>
@@ -3366,17 +3391,17 @@
       <c r="V34" s="30"/>
     </row>
     <row r="35" spans="1:22" ht="13.2">
-      <c r="A35" s="94"/>
+      <c r="A35" s="117"/>
       <c r="B35" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="100">
+      <c r="C35" s="123">
         <v>18</v>
       </c>
-      <c r="D35" s="97"/>
+      <c r="D35" s="115"/>
       <c r="E35" s="48">
         <f>E34*(1.18)</f>
-        <v>3602.4573999999989</v>
+        <v>27356.636199999997</v>
       </c>
       <c r="F35" s="37"/>
       <c r="G35" s="30"/>
@@ -3396,17 +3421,17 @@
       <c r="V35" s="30"/>
     </row>
     <row r="36" spans="1:22" ht="13.2">
-      <c r="A36" s="94"/>
+      <c r="A36" s="117"/>
       <c r="B36" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="100">
+      <c r="C36" s="123">
         <v>5</v>
       </c>
-      <c r="D36" s="97"/>
+      <c r="D36" s="115"/>
       <c r="E36" s="55">
         <f>(1+(C36/100))*E35</f>
-        <v>3782.580269999999</v>
+        <v>28724.468009999997</v>
       </c>
       <c r="F36" s="37"/>
       <c r="G36" s="30"/>
@@ -3426,7 +3451,7 @@
       <c r="V36" s="30"/>
     </row>
     <row r="37" spans="1:22" ht="13.2">
-      <c r="A37" s="95"/>
+      <c r="A37" s="118"/>
       <c r="B37" s="56" t="s">
         <v>45</v>
       </c>
@@ -3436,7 +3461,7 @@
       <c r="D37" s="107"/>
       <c r="E37" s="48">
         <f>1.667*E36</f>
-        <v>6305.5613100899982</v>
+        <v>47883.688172669994</v>
       </c>
       <c r="F37" s="37"/>
       <c r="G37" s="30"/>
@@ -3482,7 +3507,7 @@
     <row r="39" spans="1:22" ht="28.5" customHeight="1">
       <c r="A39" s="37"/>
       <c r="B39" s="108"/>
-      <c r="C39" s="92"/>
+      <c r="C39" s="109"/>
       <c r="D39" s="57"/>
       <c r="E39" s="58"/>
       <c r="F39" s="37"/>
@@ -3533,12 +3558,12 @@
       <c r="A41" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="91" t="s">
+      <c r="B41" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="109"/>
+      <c r="E41" s="109"/>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
       <c r="H41" s="30"/>
@@ -3561,12 +3586,12 @@
       <c r="A42" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="91" t="s">
+      <c r="B42" s="110" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="92"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="92"/>
+      <c r="C42" s="109"/>
+      <c r="D42" s="109"/>
+      <c r="E42" s="109"/>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
       <c r="H42" s="30"/>
@@ -26822,6 +26847,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="A38:E38"/>
@@ -26835,17 +26871,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <conditionalFormatting sqref="F1">
     <cfRule type="colorScale" priority="2">
@@ -26894,7 +26919,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -26902,7 +26927,9 @@
     <col min="1" max="2" width="25.44140625" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" customWidth="1"/>
     <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
     <col min="9" max="9" width="42.5546875" customWidth="1"/>
+    <col min="10" max="11" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21">
@@ -26918,40 +26945,40 @@
       <c r="D1" s="75" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="116" t="s">
+      <c r="F1" s="74" t="s">
         <v>169</v>
       </c>
       <c r="G1" s="75" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
       <c r="I1" s="74" t="s">
         <v>170</v>
       </c>
       <c r="J1" s="75" t="s">
-        <v>135</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="120" t="s">
+      <c r="C2" s="93" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="43">
-        <v>0.12962962962963001</v>
-      </c>
-      <c r="F2" s="117" t="s">
-        <v>36</v>
+        <v>0.13</v>
+      </c>
+      <c r="F2" s="87" t="s">
+        <v>173</v>
       </c>
       <c r="G2" s="85">
         <v>1.6E-2</v>
       </c>
-      <c r="I2" s="118" t="s">
-        <v>42</v>
+      <c r="I2" s="91" t="s">
+        <v>175</v>
       </c>
       <c r="J2" s="68">
         <v>25</v>
@@ -26961,22 +26988,22 @@
       <c r="A3" s="79" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="94" t="s">
         <v>143</v>
       </c>
       <c r="D3" s="47">
         <v>0.148148148148148</v>
       </c>
-      <c r="F3" s="117" t="s">
-        <v>37</v>
+      <c r="F3" s="87" t="s">
+        <v>174</v>
       </c>
       <c r="G3" s="66">
         <v>350</v>
       </c>
-      <c r="I3" s="118" t="s">
+      <c r="I3" s="91" t="s">
         <v>43</v>
       </c>
       <c r="J3" s="68">
@@ -26987,22 +27014,22 @@
       <c r="A4" s="79" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="94" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="47">
         <v>0.16666666666666699</v>
       </c>
-      <c r="F4" s="117" t="s">
+      <c r="F4" s="87" t="s">
         <v>38</v>
       </c>
       <c r="G4" s="66">
         <v>4</v>
       </c>
-      <c r="I4" s="118" t="s">
+      <c r="I4" s="91" t="s">
         <v>44</v>
       </c>
       <c r="J4" s="68">
@@ -27013,22 +27040,22 @@
       <c r="A5" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C5" s="94" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="47">
         <v>0.46296296296296302</v>
       </c>
-      <c r="F5" s="117" t="s">
+      <c r="F5" s="87" t="s">
         <v>39</v>
       </c>
       <c r="G5" s="66">
         <v>10</v>
       </c>
-      <c r="I5" s="119" t="s">
+      <c r="I5" s="92" t="s">
         <v>45</v>
       </c>
       <c r="J5" s="69">
@@ -27039,10 +27066,10 @@
       <c r="A6" s="79" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="94" t="s">
         <v>123</v>
       </c>
       <c r="D6" s="47">
@@ -27053,10 +27080,10 @@
       <c r="A7" s="79" t="s">
         <v>147</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="121" t="s">
+      <c r="C7" s="94" t="s">
         <v>148</v>
       </c>
       <c r="D7" s="47">
@@ -27067,10 +27094,10 @@
       <c r="A8" s="79" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="121" t="s">
+      <c r="C8" s="94" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="47">
@@ -27081,10 +27108,10 @@
       <c r="A9" s="79" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C9" s="121" t="s">
+      <c r="C9" s="94" t="s">
         <v>124</v>
       </c>
       <c r="D9" s="47">
@@ -27095,10 +27122,10 @@
       <c r="A10" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="128" t="s">
+      <c r="B10" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="121" t="s">
+      <c r="C10" s="94" t="s">
         <v>152</v>
       </c>
       <c r="D10" s="47">
@@ -27109,10 +27136,10 @@
       <c r="A11" s="79" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="121" t="s">
+      <c r="C11" s="94" t="s">
         <v>126</v>
       </c>
       <c r="D11" s="47">
@@ -27123,10 +27150,10 @@
       <c r="A12" s="79" t="s">
         <v>154</v>
       </c>
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="121" t="s">
+      <c r="C12" s="94" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="47">
@@ -27137,10 +27164,10 @@
       <c r="A13" s="79" t="s">
         <v>155</v>
       </c>
-      <c r="B13" s="128" t="s">
+      <c r="B13" s="101" t="s">
         <v>128</v>
       </c>
-      <c r="C13" s="121" t="s">
+      <c r="C13" s="94" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="47">
@@ -27151,10 +27178,10 @@
       <c r="A14" s="78" t="s">
         <v>156</v>
       </c>
-      <c r="B14" s="128" t="s">
+      <c r="B14" s="101" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="95" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="47">
@@ -27165,10 +27192,10 @@
       <c r="A15" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="B15" s="128" t="s">
+      <c r="B15" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="123" t="s">
+      <c r="C15" s="96" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="47">
@@ -27179,10 +27206,10 @@
       <c r="A16" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="128" t="s">
+      <c r="B16" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="96" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="47">
@@ -27193,10 +27220,10 @@
       <c r="A17" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="B17" s="128" t="s">
+      <c r="B17" s="101" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="96" t="s">
         <v>160</v>
       </c>
       <c r="D17" s="47">
@@ -27207,10 +27234,10 @@
       <c r="A18" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="B18" s="128" t="s">
+      <c r="B18" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="97" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="47">
@@ -27221,10 +27248,10 @@
       <c r="A19" s="81" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="128" t="s">
+      <c r="B19" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="97" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="47">
@@ -27235,10 +27262,10 @@
       <c r="A20" s="81" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="128" t="s">
+      <c r="B20" s="101" t="s">
         <v>130</v>
       </c>
-      <c r="C20" s="124" t="s">
+      <c r="C20" s="97" t="s">
         <v>26</v>
       </c>
       <c r="D20" s="47">
@@ -27249,10 +27276,10 @@
       <c r="A21" s="82" t="s">
         <v>164</v>
       </c>
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="101" t="s">
         <v>139</v>
       </c>
-      <c r="C21" s="126" t="s">
+      <c r="C21" s="99" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="47">
@@ -27263,10 +27290,10 @@
       <c r="A22" s="82" t="s">
         <v>165</v>
       </c>
-      <c r="B22" s="128" t="s">
+      <c r="B22" s="101" t="s">
         <v>139</v>
       </c>
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="99" t="s">
         <v>166</v>
       </c>
       <c r="D22" s="47">
@@ -27277,10 +27304,10 @@
       <c r="A23" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="101" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="125" t="s">
+      <c r="C23" s="98" t="s">
         <v>32</v>
       </c>
       <c r="D23" s="51">
@@ -27291,10 +27318,10 @@
       <c r="A24" s="84" t="s">
         <v>168</v>
       </c>
-      <c r="B24" s="128" t="s">
+      <c r="B24" s="101" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="127" t="s">
+      <c r="C24" s="100" t="s">
         <v>33</v>
       </c>
       <c r="D24" s="51">
@@ -27884,11 +27911,11 @@
       <c r="F16" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="114" t="s">
+      <c r="G16" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="99"/>
-      <c r="I16" s="99"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="114"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="22">
@@ -27920,11 +27947,11 @@
       <c r="F17" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="114" t="s">
+      <c r="G17" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="99"/>
-      <c r="I17" s="99"/>
+      <c r="H17" s="114"/>
+      <c r="I17" s="114"/>
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
       <c r="L17" s="22">
@@ -27956,11 +27983,11 @@
       <c r="F18" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="G18" s="114" t="s">
+      <c r="G18" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
+      <c r="H18" s="114"/>
+      <c r="I18" s="114"/>
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="22">
@@ -27992,11 +28019,11 @@
       <c r="F19" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="G19" s="114" t="s">
+      <c r="G19" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="99"/>
-      <c r="I19" s="99"/>
+      <c r="H19" s="114"/>
+      <c r="I19" s="114"/>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
       <c r="L19" s="22">
@@ -28028,11 +28055,11 @@
       <c r="F20" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="G20" s="114" t="s">
+      <c r="G20" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
+      <c r="H20" s="114"/>
+      <c r="I20" s="114"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="22">
@@ -28064,11 +28091,11 @@
       <c r="F21" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="114" t="s">
+      <c r="G21" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H21" s="99"/>
-      <c r="I21" s="97"/>
+      <c r="H21" s="114"/>
+      <c r="I21" s="115"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
       <c r="L21" s="18">
@@ -28100,11 +28127,11 @@
       <c r="F22" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="114" t="s">
+      <c r="G22" s="125" t="s">
         <v>87</v>
       </c>
-      <c r="H22" s="99"/>
-      <c r="I22" s="97"/>
+      <c r="H22" s="114"/>
+      <c r="I22" s="115"/>
       <c r="J22" s="17"/>
       <c r="K22" s="17"/>
       <c r="L22" s="18">
@@ -30171,26 +30198,26 @@
       <c r="AB30" s="9"/>
     </row>
     <row r="31" spans="1:28" ht="24" customHeight="1">
-      <c r="A31" s="115" t="s">
+      <c r="A31" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="92"/>
-      <c r="L31" s="92"/>
-      <c r="M31" s="92"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="92"/>
-      <c r="P31" s="92"/>
-      <c r="Q31" s="92"/>
-      <c r="R31" s="92"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="109"/>
+      <c r="E31" s="109"/>
+      <c r="F31" s="109"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="109"/>
+      <c r="I31" s="109"/>
+      <c r="J31" s="109"/>
+      <c r="K31" s="109"/>
+      <c r="L31" s="109"/>
+      <c r="M31" s="109"/>
+      <c r="N31" s="109"/>
+      <c r="O31" s="109"/>
+      <c r="P31" s="109"/>
+      <c r="Q31" s="109"/>
+      <c r="R31" s="109"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
       <c r="U31" s="9"/>

</xml_diff>